<commit_message>
added modern string and workitems
</commit_message>
<xml_diff>
--- a/Aljazeera.xlsx
+++ b/Aljazeera.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>18 hours ago ... Israeli 'diplomatic offensive' urges sanctions against Iran ... Push on partners to sanction Tehran comes as Israel mulls military retaliation for Iran's weekend ...</t>
+          <t>19 hours ago ... Iran's Raisi reiterates warnings as Israel mulls response to air attack. As the world calls for calm, President Raisi vows 'slightest attack' will be met with a ...</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -486,26 +486,26 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LIVE: Barcelona vs Paris Saint-Germain – Champions League ...</t>
+          <t>LIVE: Pakistan vs New Zealand – T20 international cricket | Cricket ...</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Last update 16 Apr 2024</t>
+          <t>Published On 18 Apr 2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3 hours ago ... Hello and welcome to our live coverage of Barcelona against Paris Saint-Germain in the second leg of their Champions League quarterfinal.</t>
+          <t>5 hours ago ... The sides will face each other five times as they continue their warm-up to the T20 World Cup. ... Hello and welcome to our live coverage of ...</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>LIVE:Barcelonavs</t>
+          <t>LIVE:Pakistanvs</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -516,7 +516,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Opinion | Today's latest from Al Jazeera</t>
+          <t>Nigeria | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3 days ago ... Stay on top of Opinion latest developments on the ground with Al Jazeera's fact-based news, exclusive video footage, photos and updated maps.</t>
+          <t>19 hours ago ... Why is Germany maintaining economic ties with China? German Chancellor Olaf Scholz has been on a three-day visit to China in a bid to shore up economic ties.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>OpinionToday's</t>
+          <t>NigeriaToday's</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -546,26 +546,26 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>After deadly attack, Russia's Central Asian workers report rising racism</t>
+          <t>Opinion | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Published On 9 Apr 2024</t>
+          <t>No Date</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>8 days ago ... A widely circulated screenshot of a text conversation with a taxi driver read: “Hello, if you are Tajik, cancel the order, I will not go ...</t>
+          <t>19 hours ago ... The conflict in Sudan has displaced over two million people, triggering one of the world's largest humanitarian crises. Opinion by Amitabh BeharAmitabh ...</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Afterdeadlyattack</t>
+          <t>OpinionToday's</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -576,7 +576,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Nigeria | Today's latest from Al Jazeera</t>
+          <t>Elections | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -586,12 +586,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Apr 2, 2024 ... In 2014, Rabiat and 275 other schoolgirls were abducted by Boko Haram in the town of Chibok. Dozens are still missing. Published On 14 Apr 202414 Apr 2024.</t>
+          <t>19 hours ago ... Croatians vote in election pitting the PM against the country's president ... Exit polls expected minutes after voting ends at 7pm (17:00 GMT), with official ...</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>NigeriaToday's</t>
+          <t>ElectionsToday's</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -606,26 +606,26 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Fear stalks Russia after Moscow massacre as Putin's allies play ...</t>
+          <t>Video | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Last update 25 Mar 2024</t>
+          <t>No Date</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mar 24, 2024 ... “Hello, if you are Tajik, cancel the order, I will not go with you, or I will call the traffic police, let them check your licence to ...</t>
+          <t>19 hours ago ... Dominican FM on Haiti gang violence crisis: Spillover threat? Roberto Alvarez Gil, Dominican Republic FM, discusses the effect of Haiti's criminal gang turmoil.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FearstalksRussia</t>
+          <t>VideoToday's</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Saudi Arabia | Today's latest from Al Jazeera</t>
+          <t>Listen Live to Al Jazeera | Al Jazeera</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -646,12 +646,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mar 20, 2024 ... Cristiano Ronaldo's wait for a Saudi Arabian football trophy will continue after Super Cup exit. ... Al Nassr's Cristiano Ronaldo walks on field. WTA Finals ...</t>
+          <t>2 days ago ... Live Broadcast. NEWS 30min. 2:00PM - 2:30PM. Up-to-date news and analysis from around the world.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SaudiArabia</t>
+          <t>ListenLiveto</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -666,26 +666,26 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Thomas Friedman: Dehumanisation par excellence amid a ...</t>
+          <t>Philippines | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Published On 17 Feb 2024</t>
+          <t>No Date</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Feb 16, 2024 ... A die-hard fan of Israel – to the extent that he gushes that Israel “had me at hello” – Friedman was clearly not going to be any objectively ...</t>
+          <t>2 days ago ... Filipino migrant workers in European country allege wage theft, salary deductions and passport confiscation. Published On 17 Apr 202417 Apr 2024.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ThomasFriedman:Dehumanisation</t>
+          <t>PhilippinesToday's</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -696,22 +696,22 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pakistan election 2024 updates: Blasts at candidates' offices, 24 killed</t>
+          <t>Turkey | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Last update 7 Feb 2024</t>
+          <t>No Date</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Feb 6, 2024 ... At least 24 people killed, multiple wounded as blasts target Balochistan province ahead of polls.</t>
+          <t>3 days ago ... Stay on top of Turkey latest developments on the ground with Al Jazeera's fact-based news, exclusive video footage, photos and updated maps.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Pakistanelection2024</t>
+          <t>TurkeyToday's</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -726,22 +726,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AFC Asian Cup 2023: Full match schedule</t>
+          <t>South Africa | Today's latest from Al Jazeera</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Published On 10 Jan 2024</t>
+          <t>No Date</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jan 9, 2024 ... The complete list of fixtures for the AFC Asian Cup 2023 in Qatar, with the stadiums and kick off times.</t>
+          <t>3 days ago ... Former President Jacob Zuma hopes to run for office for the opposition uMkhonto weSizwe Party (MK) in May elections. Published On 12 Apr 202412 Apr 2024.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>AFCAsianCup</t>
+          <t>SouthAfrica</t>
         </is>
       </c>
       <c r="E11" t="n">

</xml_diff>